<commit_message>
update import from file Excel - 1
</commit_message>
<xml_diff>
--- a/test-oligo.xlsx
+++ b/test-oligo.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KHACH HANG\PHU SA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEV\htdocs\bootstrap-5-ecom\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="342">
   <si>
     <t>a01</t>
   </si>
@@ -609,6 +610,447 @@
   </si>
   <si>
     <t>a146</t>
+  </si>
+  <si>
+    <t>b01</t>
+  </si>
+  <si>
+    <t>b02</t>
+  </si>
+  <si>
+    <t>b03</t>
+  </si>
+  <si>
+    <t>b04</t>
+  </si>
+  <si>
+    <t>b05</t>
+  </si>
+  <si>
+    <t>b06</t>
+  </si>
+  <si>
+    <t>b07</t>
+  </si>
+  <si>
+    <t>b08</t>
+  </si>
+  <si>
+    <t>b09</t>
+  </si>
+  <si>
+    <t>b10</t>
+  </si>
+  <si>
+    <t>b11</t>
+  </si>
+  <si>
+    <t>b12</t>
+  </si>
+  <si>
+    <t>b13</t>
+  </si>
+  <si>
+    <t>b14</t>
+  </si>
+  <si>
+    <t>b15</t>
+  </si>
+  <si>
+    <t>b16</t>
+  </si>
+  <si>
+    <t>b17</t>
+  </si>
+  <si>
+    <t>b18</t>
+  </si>
+  <si>
+    <t>b19</t>
+  </si>
+  <si>
+    <t>b20</t>
+  </si>
+  <si>
+    <t>b21</t>
+  </si>
+  <si>
+    <t>b22</t>
+  </si>
+  <si>
+    <t>b23</t>
+  </si>
+  <si>
+    <t>b24</t>
+  </si>
+  <si>
+    <t>b25</t>
+  </si>
+  <si>
+    <t>b26</t>
+  </si>
+  <si>
+    <t>b27</t>
+  </si>
+  <si>
+    <t>b28</t>
+  </si>
+  <si>
+    <t>b29</t>
+  </si>
+  <si>
+    <t>b30</t>
+  </si>
+  <si>
+    <t>b31</t>
+  </si>
+  <si>
+    <t>b32</t>
+  </si>
+  <si>
+    <t>b33</t>
+  </si>
+  <si>
+    <t>b34</t>
+  </si>
+  <si>
+    <t>b35</t>
+  </si>
+  <si>
+    <t>b36</t>
+  </si>
+  <si>
+    <t>b37</t>
+  </si>
+  <si>
+    <t>b38</t>
+  </si>
+  <si>
+    <t>b39</t>
+  </si>
+  <si>
+    <t>b40</t>
+  </si>
+  <si>
+    <t>b41</t>
+  </si>
+  <si>
+    <t>b42</t>
+  </si>
+  <si>
+    <t>b43</t>
+  </si>
+  <si>
+    <t>b44</t>
+  </si>
+  <si>
+    <t>b45</t>
+  </si>
+  <si>
+    <t>b46</t>
+  </si>
+  <si>
+    <t>b47</t>
+  </si>
+  <si>
+    <t>b48</t>
+  </si>
+  <si>
+    <t>b49</t>
+  </si>
+  <si>
+    <t>b50</t>
+  </si>
+  <si>
+    <t>b51</t>
+  </si>
+  <si>
+    <t>b52</t>
+  </si>
+  <si>
+    <t>b53</t>
+  </si>
+  <si>
+    <t>b54</t>
+  </si>
+  <si>
+    <t>b55</t>
+  </si>
+  <si>
+    <t>b56</t>
+  </si>
+  <si>
+    <t>b57</t>
+  </si>
+  <si>
+    <t>b58</t>
+  </si>
+  <si>
+    <t>b59</t>
+  </si>
+  <si>
+    <t>b60</t>
+  </si>
+  <si>
+    <t>b61</t>
+  </si>
+  <si>
+    <t>b62</t>
+  </si>
+  <si>
+    <t>b63</t>
+  </si>
+  <si>
+    <t>b64</t>
+  </si>
+  <si>
+    <t>b65</t>
+  </si>
+  <si>
+    <t>b66</t>
+  </si>
+  <si>
+    <t>b67</t>
+  </si>
+  <si>
+    <t>b68</t>
+  </si>
+  <si>
+    <t>b69</t>
+  </si>
+  <si>
+    <t>b70</t>
+  </si>
+  <si>
+    <t>b71</t>
+  </si>
+  <si>
+    <t>b72</t>
+  </si>
+  <si>
+    <t>b73</t>
+  </si>
+  <si>
+    <t>b74</t>
+  </si>
+  <si>
+    <t>b75</t>
+  </si>
+  <si>
+    <t>b76</t>
+  </si>
+  <si>
+    <t>b77</t>
+  </si>
+  <si>
+    <t>b78</t>
+  </si>
+  <si>
+    <t>b79</t>
+  </si>
+  <si>
+    <t>b80</t>
+  </si>
+  <si>
+    <t>b81</t>
+  </si>
+  <si>
+    <t>b82</t>
+  </si>
+  <si>
+    <t>b83</t>
+  </si>
+  <si>
+    <t>b84</t>
+  </si>
+  <si>
+    <t>b85</t>
+  </si>
+  <si>
+    <t>b86</t>
+  </si>
+  <si>
+    <t>b87</t>
+  </si>
+  <si>
+    <t>b88</t>
+  </si>
+  <si>
+    <t>b89</t>
+  </si>
+  <si>
+    <t>b90</t>
+  </si>
+  <si>
+    <t>b91</t>
+  </si>
+  <si>
+    <t>b92</t>
+  </si>
+  <si>
+    <t>b93</t>
+  </si>
+  <si>
+    <t>b94</t>
+  </si>
+  <si>
+    <t>b95</t>
+  </si>
+  <si>
+    <t>b96</t>
+  </si>
+  <si>
+    <t>b97</t>
+  </si>
+  <si>
+    <t>b98</t>
+  </si>
+  <si>
+    <t>b99</t>
+  </si>
+  <si>
+    <t>b100</t>
+  </si>
+  <si>
+    <t>b101</t>
+  </si>
+  <si>
+    <t>b102</t>
+  </si>
+  <si>
+    <t>b103</t>
+  </si>
+  <si>
+    <t>b104</t>
+  </si>
+  <si>
+    <t>b105</t>
+  </si>
+  <si>
+    <t>b106</t>
+  </si>
+  <si>
+    <t>b107</t>
+  </si>
+  <si>
+    <t>b108</t>
+  </si>
+  <si>
+    <t>b109</t>
+  </si>
+  <si>
+    <t>b110</t>
+  </si>
+  <si>
+    <t>b111</t>
+  </si>
+  <si>
+    <t>b112</t>
+  </si>
+  <si>
+    <t>b113</t>
+  </si>
+  <si>
+    <t>b114</t>
+  </si>
+  <si>
+    <t>b115</t>
+  </si>
+  <si>
+    <t>b116</t>
+  </si>
+  <si>
+    <t>b117</t>
+  </si>
+  <si>
+    <t>b118</t>
+  </si>
+  <si>
+    <t>b119</t>
+  </si>
+  <si>
+    <t>b120</t>
+  </si>
+  <si>
+    <t>b121</t>
+  </si>
+  <si>
+    <t>b122</t>
+  </si>
+  <si>
+    <t>b123</t>
+  </si>
+  <si>
+    <t>b124</t>
+  </si>
+  <si>
+    <t>b125</t>
+  </si>
+  <si>
+    <t>b126</t>
+  </si>
+  <si>
+    <t>b127</t>
+  </si>
+  <si>
+    <t>b128</t>
+  </si>
+  <si>
+    <t>b129</t>
+  </si>
+  <si>
+    <t>b130</t>
+  </si>
+  <si>
+    <t>b131</t>
+  </si>
+  <si>
+    <t>b132</t>
+  </si>
+  <si>
+    <t>b133</t>
+  </si>
+  <si>
+    <t>b134</t>
+  </si>
+  <si>
+    <t>b135</t>
+  </si>
+  <si>
+    <t>b136</t>
+  </si>
+  <si>
+    <t>b137</t>
+  </si>
+  <si>
+    <t>b138</t>
+  </si>
+  <si>
+    <t>b139</t>
+  </si>
+  <si>
+    <t>b140</t>
+  </si>
+  <si>
+    <t>b141</t>
+  </si>
+  <si>
+    <t>b142</t>
+  </si>
+  <si>
+    <t>b143</t>
+  </si>
+  <si>
+    <t>b144</t>
+  </si>
+  <si>
+    <t>b145</t>
+  </si>
+  <si>
+    <t>b146</t>
+  </si>
+  <si>
+    <t>b147</t>
   </si>
 </sst>
 </file>
@@ -929,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B147" sqref="A1:C147"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B45" sqref="A1:C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2114,4 +2556,1192 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C147"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection sqref="A1:A147"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>210</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>211</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>215</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>216</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>217</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>218</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>219</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>220</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>221</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>222</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>223</v>
+      </c>
+      <c r="B29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>224</v>
+      </c>
+      <c r="B30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>225</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>226</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>227</v>
+      </c>
+      <c r="B33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>228</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>229</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>230</v>
+      </c>
+      <c r="B36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>231</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>232</v>
+      </c>
+      <c r="B38" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>233</v>
+      </c>
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>234</v>
+      </c>
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>235</v>
+      </c>
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>236</v>
+      </c>
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>237</v>
+      </c>
+      <c r="B43" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>238</v>
+      </c>
+      <c r="B44" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>239</v>
+      </c>
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>240</v>
+      </c>
+      <c r="B46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>241</v>
+      </c>
+      <c r="B47" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>242</v>
+      </c>
+      <c r="B48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>243</v>
+      </c>
+      <c r="B49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>244</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>245</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>246</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>247</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>248</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>249</v>
+      </c>
+      <c r="B55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>250</v>
+      </c>
+      <c r="B56" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>251</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>252</v>
+      </c>
+      <c r="B58" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>253</v>
+      </c>
+      <c r="B59" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>254</v>
+      </c>
+      <c r="B60" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>255</v>
+      </c>
+      <c r="B61" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>256</v>
+      </c>
+      <c r="B62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>257</v>
+      </c>
+      <c r="B63" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>259</v>
+      </c>
+      <c r="B65" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>260</v>
+      </c>
+      <c r="B66" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>261</v>
+      </c>
+      <c r="B67" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>262</v>
+      </c>
+      <c r="B68" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>263</v>
+      </c>
+      <c r="B69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>264</v>
+      </c>
+      <c r="B70" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>265</v>
+      </c>
+      <c r="B71" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>266</v>
+      </c>
+      <c r="B72" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>267</v>
+      </c>
+      <c r="B73" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>268</v>
+      </c>
+      <c r="B74" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>269</v>
+      </c>
+      <c r="B75" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>270</v>
+      </c>
+      <c r="B76" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>271</v>
+      </c>
+      <c r="B77" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>272</v>
+      </c>
+      <c r="B78" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>273</v>
+      </c>
+      <c r="B79" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>274</v>
+      </c>
+      <c r="B80" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>275</v>
+      </c>
+      <c r="B81" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>276</v>
+      </c>
+      <c r="B82" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>277</v>
+      </c>
+      <c r="B83" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>278</v>
+      </c>
+      <c r="B84" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>279</v>
+      </c>
+      <c r="B85" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>280</v>
+      </c>
+      <c r="B86" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>281</v>
+      </c>
+      <c r="B87" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>282</v>
+      </c>
+      <c r="B88" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>283</v>
+      </c>
+      <c r="B89" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>284</v>
+      </c>
+      <c r="B90" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>285</v>
+      </c>
+      <c r="B91" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>286</v>
+      </c>
+      <c r="B92" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>287</v>
+      </c>
+      <c r="B93" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>288</v>
+      </c>
+      <c r="B94" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>289</v>
+      </c>
+      <c r="B95" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>290</v>
+      </c>
+      <c r="B96" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>291</v>
+      </c>
+      <c r="B97" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>292</v>
+      </c>
+      <c r="B98" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>293</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>294</v>
+      </c>
+      <c r="B100" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>295</v>
+      </c>
+      <c r="B101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>296</v>
+      </c>
+      <c r="B102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>297</v>
+      </c>
+      <c r="B103" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>298</v>
+      </c>
+      <c r="B104" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>299</v>
+      </c>
+      <c r="B105" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>300</v>
+      </c>
+      <c r="B106" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>301</v>
+      </c>
+      <c r="B107" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>302</v>
+      </c>
+      <c r="B108" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>303</v>
+      </c>
+      <c r="B109" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>304</v>
+      </c>
+      <c r="B110" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>305</v>
+      </c>
+      <c r="B111" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>306</v>
+      </c>
+      <c r="B112" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>308</v>
+      </c>
+      <c r="B114" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>309</v>
+      </c>
+      <c r="B115" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>310</v>
+      </c>
+      <c r="B116" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>311</v>
+      </c>
+      <c r="B117" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>312</v>
+      </c>
+      <c r="B118" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>313</v>
+      </c>
+      <c r="B119" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>314</v>
+      </c>
+      <c r="B120" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>315</v>
+      </c>
+      <c r="B121" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>316</v>
+      </c>
+      <c r="B122" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>317</v>
+      </c>
+      <c r="B123" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>318</v>
+      </c>
+      <c r="B124" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>319</v>
+      </c>
+      <c r="B125" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>320</v>
+      </c>
+      <c r="B126" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>321</v>
+      </c>
+      <c r="B127" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>322</v>
+      </c>
+      <c r="B128" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>323</v>
+      </c>
+      <c r="B129" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>324</v>
+      </c>
+      <c r="B130" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>325</v>
+      </c>
+      <c r="B131" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>326</v>
+      </c>
+      <c r="B132" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>327</v>
+      </c>
+      <c r="B133" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>328</v>
+      </c>
+      <c r="B134" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>329</v>
+      </c>
+      <c r="B135" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>330</v>
+      </c>
+      <c r="B136" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>331</v>
+      </c>
+      <c r="B137" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>332</v>
+      </c>
+      <c r="B138" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>333</v>
+      </c>
+      <c r="B139" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>334</v>
+      </c>
+      <c r="B140" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>335</v>
+      </c>
+      <c r="B141" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>336</v>
+      </c>
+      <c r="B142" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>337</v>
+      </c>
+      <c r="B143" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>338</v>
+      </c>
+      <c r="B144" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>339</v>
+      </c>
+      <c r="B145" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>340</v>
+      </c>
+      <c r="B146" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>341</v>
+      </c>
+      <c r="B147" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>